<commit_message>
added method for verify text and color
</commit_message>
<xml_diff>
--- a/src/main/java/resources/TestData.xlsx
+++ b/src/main/java/resources/TestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{47E3030B-CE63-4658-964D-3EC31374988A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6ACCE07E-7AF8-4FEC-9975-5F2FED3FE352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17304" windowHeight="12312" xr2:uid="{044AC0F2-83BB-4732-B581-3D1C0166C49B}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17328" windowHeight="13224" activeTab="1" xr2:uid="{044AC0F2-83BB-4732-B581-3D1C0166C49B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:S13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Ankur</t>
   </si>
@@ -45,6 +46,21 @@
   </si>
   <si>
     <t>jfjwei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>PIN Code</t>
   </si>
 </sst>
 </file>
@@ -398,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D9F959-AFA1-468B-AA49-C7D072826C79}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -451,4 +467,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B4E7CC-93DF-4BCB-A58C-A7FE59271853}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>